<commit_message>
Updated attributes to inputs, added cosmetic changes in overlay.rb and updated the excel sheet
Signed-off-by: karikarshivani <karikarshivani@gmail.com>
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-aws-foundations-cis-overlay.xlsx
+++ b/cms-ars-3.1-moderate-aws-foundations-cis-overlay.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\ALL_SHEETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\AWS\Overlay\cms-ars-3.1-moderate-aws-foundations-cis-overlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DC8D12-67E5-43DB-A7C2-F241FB765EBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-552" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45975" yWindow="-555" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assessment Data'!$A$1:$G$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assessment Data'!$B$1:$H$50</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="266">
   <si>
     <t>Weakness Description</t>
   </si>
@@ -134,10 +133,6 @@
   </si>
   <si>
     <t>Low</t>
-  </si>
-  <si>
-    <t>(Test 1.24) -  Ensure IAM policies that allow full '*:*' administrative privileges
-are not created</t>
   </si>
   <si>
     <t>Ensure IAM policies that allow full '*:*' administrative privileges
@@ -188,52 +183,6 @@
  'aws iam detach-role-policy --role-name __ --policy-arn __
 '
 </t>
-  </si>
-  <si>
-    <t>(Test 3.15) -  Ensure appropriate subscribers to each SNS topic</t>
-  </si>
-  <si>
-    <t>Ensure appropriate subscribers to each SNS topic</t>
-  </si>
-  <si>
-    <t>AWS Simple Notification Service (SNS) is a web service that can
-publish messages from an application and immediately deliver them to
-subscribers or other applications. Subscribers are clients interested in
-receiving notifications from topics of interest; they can subscribe to a topic
-or be subscribed by the topic owner. When publishers have information or
-updates to notify their subscribers about, they can publish a message to the
-topic - which immediately triggers Amazon SNS to deliver the message to all
-applicable subscribers. It is recommended that the list of subscribers to given
-topics be periodically reviewed for appropriateness.</t>
-  </si>
-  <si>
-    <t>Perform the following to ensure appropriate subscribers:
-'Via the AWS Management console:
- 'Sign in to the AWS Management Console and open the SNS console at
-https://console.aws.amazon.com/sns/ [https://console.aws.amazon.com/sns/]
-* Click on Topics in the left navigation pane
-* Evaluate Topics by clicking on the value within the ARN column
-* Within a selected Topic evaluate:
-* Topic owner
-* Region
-* Within the Subscriptions_ _section evaluate:
-* _Subscription ID_
-* _Protocol_
-* _Endpoint_
-* _Subscriber_ (Account ID)
-'Via CLI:
-'aws sns list-topics
-aws sns list-subscriptions-by-topic --topic-arn __</t>
-  </si>
-  <si>
-    <t>Perform the following to remove undesired subscriptions:
-'Via Management Console
- 'Sign in to the AWS Management Console and open the SNS console at
-https://console.aws.amazon.com/sns/ [https://console.aws.amazon.com/sns/]
-* Click on Subscriptions in the left navigation pane
-* For any undesired subscription, select the corresponding checkboxes
-* Click Actions
-* Click Delete Subscriptions</t>
   </si>
   <si>
     <t>(Test 1.12) -  Ensure no root account access key exists</t>
@@ -337,10 +286,6 @@
 </t>
   </si>
   <si>
-    <t>(Test 1.23) -  Do not setup access keys during initial user setup for all IAM users
-that have a console password</t>
-  </si>
-  <si>
     <t>Do not setup access keys during initial user setup for all IAM users
 that have a console password</t>
   </si>
@@ -395,311 +340,6 @@
 profile but have not been used.
 'Via CLI
 'aws iam delete-access-key</t>
-  </si>
-  <si>
-    <t>(Test 1.18) -  Ensure IAM Master and IAM Manager roles are active</t>
-  </si>
-  <si>
-    <t>Ensure IAM Master and IAM Manager roles are active</t>
-  </si>
-  <si>
-    <t>Ensure IAM Master and IAM Manager roles are in place for IAM
-administration and assignment of administrative permissions for other services
-to other roles.
-'An IAM role is conceptually 'a container of permissions resembling a user
-account which cannot be directly logged into, but which must instead be assumed
-from an existing user account which has appropriate permissions to do so', in
-the manner of roles in Unix Role-Based Access Control (RBAC). In AWS, roles can
-also be assigned to EC2 instances and Lambda functions.
-Control over IAM, which is also defined and mediated by a number of
-fine-grained permissions, should be divided between a number of roles, such
-that no individual user in a production account has full control over IAM.</t>
-  </si>
-  <si>
-    <t>Using the Amazon unified CLI, from a user or role which has the
-iam:ListRoles and iam:GetRolePolicy permissions:
-List the configured roles:
-'aws iam list-roles --query 'Roles[*].{RoleName:RoleName, Arn:Arn}'
-'The output should contain entries with 'RoleName': '__'
-and 'Rolename': '__'
-Examine the permissions associated with each of these roles:
-'aws iam get-role-policy --role-name __
-'aws iam get-role-policy --role-name __
-The __ role should include the following Actions with an
-Allow effect:
-iam:AttachRolePolicy
-iam:CreateGroup
-iam:CreatePolicy
-iam:CreatePolicyVersion
-iam:CreateRole
-iam:CreateUser
-iam:DeleteGroup
-iam:DeletePolicy
-iam:DeletePolicyVersion
-iam:DeleteRole
-iam:DeleteRolePolicy
-iam:DeleteUser
-iam:PutRolePolicy
-iam:GetPolicy
-iam:GetPolicyVersion
-iam:GetRole
-iam:GetRolePolicy
-iam:GetUser
-iam:GetUserPolicy
-iam:ListEntitiesForPolicy
-iam:ListGroupPolicies
-iam:ListGroups
-iam:ListGroupsForUser
-iam:ListPolicies
-iam:ListPoliciesGrantingServiceAccess
-iam:ListPolicyVersions
-iam:ListRolePolicies
-iam:ListAttachedGroupPolicies
-iam:ListAttachedRolePolicies
-iam:ListAttachedUserPolicies
-iam:ListRoles
-iam:ListUsers
-and the following Actions with a Deny effect:
-iam:AddUserToGroup
-iam:AttachGroupPolicy
-iam:DeleteGroupPolicy
-iam:DeleteUserPolicy
-iam:DetachGroupPolicy
-iam:DetachRolePolicy
-iam:DetachUserPolicy
-iam:PutGroupPolicy
-iam:PutUserPolicy
-iam:RemoveUserFromGroup
-iam:UpdateGroup
-iam:UpdateAssumeRolePolicy
-iam:UpdateUser
-The __ role should include the following Actions with an
-Allow effect:
-iam:AddUserToGroup
-iam:AttachGroupPolicy
-iam:DeleteGroupPolicy
-iam:DeleteUserPolicy
-iam:DetachGroupPolicy
-iam:DetachRolePolicy
-iam:DetachUserPolicy
-iam:PutGroupPolicy
-iam:PutUserPolicy
-iam:RemoveUserFromGroup
-iam:UpdateGroup
-iam:UpdateAssumeRolePolicy
-iam:UpdateUser
-iam:GetPolicy
-iam:GetPolicyVersion
-iam:GetRole
-iam:GetRolePolicy
-iam:GetUser
-iam:GetUserPolicy
-iam:ListEntitiesForPolicy
-iam:ListGroupPolicies
-iam:ListGroups
-iam:ListGroupsForUser
-iam:ListPolicies
-iam:ListPoliciesGrantingServiceAccess
-iam:ListPolicyVersions
-iam:ListRolePolicies
-iam:ListAttachedGroupPolicies
-iam:ListAttachedRolePolicies
-iam:ListAttachedUserPolicies
-iam:ListRoles
-iam:ListUsers
-and the following Actions with a Deny effect:
-iam: AttachRolePolicy
-iam:CreateGroup
-iam:CreatePolicy
-iam:CreatePolicyVersion
-iam:CreateRole
-iam:CreateUser
-iam:DeleteGroup
-iam:DeletePolicy
-iam:DeletePolicyVersion
-iam:DeleteRole
-iam:DeleteRolePolicy
-iam:DeleteUser
-iam:PutRolePolicy
-Other iam:* Actions may be included in these policies as needed.
-Both policies should also be limited by a Condition that MFA authentication is
-in effect, by containing:
-'Condition': {'Bool': {'aws:MultiFactorAuthPresent': 'true'}}
-in the Allow effect section (provided IAM Federation has not been configured).
-Each role needs to be assumable by at least one user or group:
-'aws iam get-role --role-name __
-'aws iam get-role --role-name __
-'should display the AssumeRolePolicyDocument indicating which users and groups
-are able to assume the roles. No user or group should be able to assume both
-roles.</t>
-  </si>
-  <si>
-    <t>Using the Amazon unified CLI, from a user or role which has the
-iam:CreateRole, iam:CreatePolicy and iam:PutRolePolicy permissions:
-'aws iam create-role --role-name __
-'aws iam create-role --role-name __
-'aws iam put-role-policy --role-name __ --policy-name
-__ --policy-document
-file://IAM-Manager-policy.json
-'aws iam put-role-policy --role-name __ --policy-name
-__ --policy-document
-file://IAM-Master-policy.json
-'where IAM-Master-policy.json contains:
-'{
-' 'Version': '2012-10-17',
-' 'Statement': [{
-' 'Action': [
-' 'iam:CreateGroup',
-''iam:CreatePolicy',
-''iam:CreatePolicyVersion',
-''iam:CreateRole',
-''iam:CreateUser',
-''iam:DeleteGroup',
-''iam:DeletePolicy',
-''iam:DeletePolicyVersion',
-''iam:DeleteRole',
-''iam:DeleteRolePolicy',
-''iam:DeleteUser',
-''iam:PutRolePolicy',
-''iam:GetPolicy',
-''iam:GetPolicyVersion',
-''iam:GetRole',
-''iam:GetRolePolicy',
-''iam:GetUser',
-''iam:GetUserPolicy',
-''iam:ListEntitiesForPolicy',
-''iam:ListGroupPolicies',
-''iam:ListGroups',
-''iam:ListGroupsForUser',
-''iam:ListPolicies',
-''iam:ListPoliciesGrantingServiceAccess',
-''iam:ListPolicyVersions',
-''iam:ListRolePolicies',
-''iam:ListAttachedGroupPolicies',
-''iam:ListAttachedRolePolicies',
-''iam:ListAttachedUserPolicies',
-''iam:ListRoles',
-''iam:ListUsers'
-' ],
-' 'Effect': 'Allow',
-' 'Resource': '*',
-' 'Condition': {'Bool': {'aws:MultiFactorAuthPresent': 'true'}}
-' }],
-' 'Action': [
-''iam:AddUserToGroup',
-''iam:AttachGroupPolicy',
-''iam:DeleteGroupPolicy',
-''iam:DeleteUserPolicy',
-''iam:DetachGroupPolicy',
-''iam:DetachRolePolicy',
-''iam:DetachUserPolicy',
-''iam:PutGroupPolicy',
-''iam:PutUserPolicy',
-''iam:RemoveUserFromGroup',
-''iam:UpdateGroup',
-''iam:UpdateAssumeRolePolicy',
-''iam:UpdateUser'
-' ],
-' 'Effect': 'Deny',
-' 'Resource': '*'
-' }]
-'}
-'and where IAM-Manager-policy.json contains:
-'{
-' 'Version': '2012-10-17',
-' 'Statement': [{
-' 'Action': [
-''iam:AddUserToGroup',
-''iam:AttachGroupPolicy',
-''iam:DeleteGroupPolicy',
-''iam:DeleteUserPolicy',
-''iam:DetachGroupPolicy',
-''iam:DetachRolePolicy',
-''iam:DetachUserPolicy',
-''iam:PutGroupPolicy',
-''iam:PutUserPolicy',
-''iam:RemoveUserFromGroup',
-''iam:UpdateGroup',
-''iam:UpdateAssumeRolePolicy',
-''iam:UpdateUser',
-''iam:GetPolicy',
-''iam:GetPolicyVersion',
-''iam:GetRole',
-''iam:GetRolePolicy',
-''iam:GetUser',
-''iam:GetUserPolicy',
-''iam:ListEntitiesForPolicy',
-''iam:ListGroupPolicies',
-''iam:ListGroups',
-''iam:ListGroupsForUser',
-''iam:ListPolicies',
-''iam:ListPoliciesGrantingServiceAccess',
-''iam:ListPolicyVersions',
-''iam:ListRolePolicies',
-''iam:ListAttachedGroupPolicies',
-''iam:ListAttachedRolePolicies',
-''iam:ListAttachedUserPolicies',
-''iam:ListRoles',
-''iam:ListUsers'
-' ],
-' 'Effect': 'Allow',
-' 'Resource': '*',
-' 'Condition': {'Bool': {'aws:MultiFactorAuthPresent': 'true'}}
-' }],
-' 'Action': [
-' 'iam:CreateGroup',
-''iam:CreatePolicy',
-''iam:CreatePolicyVersion',
-''iam:CreateRole',
-''iam:CreateUser',
-''iam:DeleteGroup',
-''iam:DeletePolicy',
-''iam:DeletePolicyVersion',
-''iam:DeleteRole',
-''iam:DeleteRolePolicy',
-''iam:DeleteUser',
-''iam:PutRolePolicy'
-' ],
-' 'Effect': 'Deny',
-' 'Resource': '*'
-' }]
-'}
-'Note that each of IAM-Manager-policy.json and IAM-Master-policy.json can
-contain other iam:* permissions in either Allow or Deny Action lists, depending
-on what other requirements are in place in the account.
-'Each of these roles needs to be assumable by a different user or group.
-'For appropriate users or groups (groups are recommended):
-'aws iam put-user-policy --user-name __ --policy-name
-__ --policy-document
-file://Assume-IAM-Master.json
-'aws iam put-user-policy --user-name __ --policy-name
-__ --policy-document
-file://Assume-IAM-Manager.json
-'or
-'aws iam put-group-policy --group-name __  --policy-name
-__ --policy-document
-file://Assume-IAM-Master.json
-'aws iam put-group-policy --group-name __ --policy-name
-_ _--policy-document
-file://Assume-IAM-Manager.json
-'where Assume-IAM-Master.json is:
-'{
-' 'Version': '2012-10-17',
-' 'Statement': {
-' 'Effect': 'Allow',
-' 'Action': 'sts:AssumeRole',
-' 'Resource': 'arn:aws:iam::__:role/'
-' }
-'}
-'and Assume-IAM-Manager.json is:
-'{
-' 'Version': '2012-10-17',
-' 'Statement': {
-' 'Effect': 'Allow',
-' 'Action': 'sts:AssumeRole',
-' 'Resource': 'arn:aws:iam:::role/'
-' }
-'}</t>
   </si>
   <si>
     <t>(Test 3.3) -  Ensure a log metric filter and alarm exist for usage of 'root' account</t>
@@ -1181,67 +821,6 @@
 * Click Save to save the ACL.
 * If the Edit bucket policy button is present, click it.
 * Remove any Statement having an Effect set to Allow and a Principal set to *.</t>
-  </si>
-  <si>
-    <t>AU-12</t>
-  </si>
-  <si>
-    <t>(Test 1.17) -  Enable detailed billing</t>
-  </si>
-  <si>
-    <t>Enable detailed billing</t>
-  </si>
-  <si>
-    <t>Enable Detailed Billing to cause the generation of a log record for
-every event or hourly ongoing activity which incurs cost in an AWS account.
-These records are aggregated into CSV files of hourly records, and written to
-an S3 bucket. A CSV (Comma Separated Values) file of billing records is written
-at least every 24 hours; writing of files is often more frequent.</t>
-  </si>
-  <si>
-    <t>There is currently no AWS CLI support for this operation, so it
-is necessary to use the Management Console.
-As a user with IAM permission to read billing information
-(aws-portal:ViewBilling):
-* Sign in to the AWS Management Console and open the Billing and Cost
-Management console at https://console.aws.amazon.com/billing/home#/.
-* On the navigation pane, choose Preferences.
-* Verify whether the 'Receive Billing Reports' check box is ticked. If it is
-not, billing reports are not being generated.</t>
-  </si>
-  <si>
-    <t>There is currently no AWS CLI support for this operation, so it
-is necessary to use the Management Console.
-'As a user with IAM permission to read and write billing information
-(aws-portal:*Billing):
-* Sign in to the AWS Management Console and open the Billing and Cost
-Management console at https://console.aws.amazon.com/billing/home#/
-[https://console.aws.amazon.com/billing/home#/].
-* On the navigation pane, choose Preferences.
-* Select the Receive Billing Reports check box.
-* Designate the Amazon S3 bucket __ where you want AWS to
-publish your detailed billing reports.
-* Ensure that policy allows read access only to appropriate groups of users
-(finance, auditors, etc). For appropriate groups in IAM who you want to have
-read access, include the following policy element:
-' 'Statement':[
-' {
-' 'Effect':'Allow',
-' 'Action':[
-' 's3:GetObject',
-' 's3:GetObjectVersion',
-' 's3:GetBucketLocation'
-' ],
-' 'Resource':'arn:aws:s3:::__/*'
-' }
-' ]
-* After your S3 bucket has been verified, under Report, select the check boxes
-for the reports that you want to receive.
-* Choose Save preferences
-* Detailed billing reports can take up to 24 hours to start being generated.
-Wait &gt;24 hours, and examine your designated S3 bucket to verify that files with
-names of the form (eg) -.csv.zip
-are being generated.</t>
   </si>
   <si>
     <t>IA-02</t>
@@ -1577,9 +1156,6 @@
 </t>
   </si>
   <si>
-    <t>(Test 1.20) -  Ensure security contact information is registered</t>
-  </si>
-  <si>
     <t>Ensure security contact information is registered</t>
   </si>
   <si>
@@ -1604,9 +1180,6 @@
 * Enter contact information in the Security section
 'Note: Consider specifying an internal email distribution list to ensure emails
 are regularly monitored by more than one individual.</t>
-  </si>
-  <si>
-    <t>(Test 1.19) -  Maintain current contact details</t>
   </si>
   <si>
     <t>Maintain current contact details</t>
@@ -1945,10 +1518,6 @@
   </si>
   <si>
     <t>IR-07</t>
-  </si>
-  <si>
-    <t>(Test 1.22) -  Ensure a support role has been created to manage incidents with AWS
-Support</t>
   </si>
   <si>
     <t>Ensure a support role has been created to manage incidents with AWS
@@ -1998,9 +1567,6 @@
     <t>SC-07</t>
   </si>
   <si>
-    <t>(Test 4.5) -  Ensure routing tables for VPC peering are 'least access'</t>
-  </si>
-  <si>
     <t>Ensure routing tables for VPC peering are 'least access'</t>
   </si>
   <si>
@@ -2075,9 +1641,6 @@
 * Identify the rules to be removed
 * Click the x in the Remove column
 * Click Save</t>
-  </si>
-  <si>
-    <t>(Test 4.4) -  Ensure the default security group of every VPC restricts all traffic</t>
   </si>
   <si>
     <t>Ensure the default security group of every VPC restricts all traffic</t>
@@ -2232,10 +1795,6 @@
   </si>
   <si>
     <t>SC-28</t>
-  </si>
-  <si>
-    <t>(Test 1.21) -  Ensure IAM instance roles are used for AWS resource access from
-instances</t>
   </si>
   <si>
     <t>Ensure IAM instance roles are used for AWS resource access from
@@ -2734,9 +2293,6 @@
 </t>
   </si>
   <si>
-    <t>(Test 4.3) -  Ensure VPC flow logging is enabled in all VPCs</t>
-  </si>
-  <si>
     <t>Ensure VPC flow logging is enabled in all VPCs</t>
   </si>
   <si>
@@ -3096,11 +2652,45 @@
   <si>
     <t>Description</t>
   </si>
+  <si>
+    <t>(Test 1.17) -  Maintain current contact details</t>
+  </si>
+  <si>
+    <t>(Test 1.18) -  Ensure security contact information is registered</t>
+  </si>
+  <si>
+    <t>(Test 1.19) -  Ensure IAM instance roles are used for AWS resource access from
+instances</t>
+  </si>
+  <si>
+    <t>(Test 1.20) -  Ensure a support role has been created to manage incidents with AWS
+Support</t>
+  </si>
+  <si>
+    <t>(Test 1.21) -  Do not setup access keys during initial user setup for all IAM users
+that have a console password</t>
+  </si>
+  <si>
+    <t>(Test 1.22) -  Ensure IAM policies that allow full '*:*' administrative privileges
+are not created</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>(Test 2.9) -  Ensure VPC flow logging is enabled in all VPCs</t>
+  </si>
+  <si>
+    <t>(Test 4.3) -  Ensure the default security group of every VPC restricts all traffic</t>
+  </si>
+  <si>
+    <t>(Test 4.4) -  Ensure routing tables for VPC peering are 'least access'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3159,7 +2749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3173,7 +2763,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3514,1249 +3110,1338 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.046875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="50" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.84765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.94921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.046875" style="1"/>
-    <col min="6" max="6" width="34.546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1484375" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="50.046875" style="1"/>
+    <col min="1" max="1" width="3" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50" style="1"/>
+    <col min="7" max="7" width="34.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="50" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.6">
-      <c r="A1" s="2" t="s">
-        <v>276</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="265.2" x14ac:dyDescent="0.6">
-      <c r="A2" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="267.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="378" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="267.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="362.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="C34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A4" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H47" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="48" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A6" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="405.6" x14ac:dyDescent="0.6">
-      <c r="A8" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A12" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="265.2" x14ac:dyDescent="0.6">
-      <c r="A14" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A15" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A16" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A20" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A21" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A22" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="374.4" x14ac:dyDescent="0.6">
-      <c r="A24" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="390" x14ac:dyDescent="0.6">
-      <c r="A25" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="358.8" x14ac:dyDescent="0.6">
-      <c r="A31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A32" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A33" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A34" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A35" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A36" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A37" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A38" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A39" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A41" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A43" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A44" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A45" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A46" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A47" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="312" x14ac:dyDescent="0.6">
-      <c r="A49" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="312" x14ac:dyDescent="0.6">
-      <c r="A50" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A51" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="409.5" x14ac:dyDescent="0.6">
-      <c r="A52" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="358.8" x14ac:dyDescent="0.6">
-      <c r="A53" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>184</v>
+      <c r="H50" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G53" xr:uid="{D176E819-3BF2-44A8-98E0-6B95184F970E}"/>
+  <autoFilter ref="B1:H50">
+    <sortState ref="B2:H51">
+      <sortCondition ref="B1:B51"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:H50">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>